<commit_message>
added two board versions
</commit_message>
<xml_diff>
--- a/hardware/rev_e/board/v_spec/monoxalyze.xlsx
+++ b/hardware/rev_e/board/v_spec/monoxalyze.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="199">
   <si>
     <t>Part</t>
   </si>
@@ -203,6 +203,15 @@
     <t>C21</t>
   </si>
   <si>
+    <t>C22</t>
+  </si>
+  <si>
+    <t>0403_CAP</t>
+  </si>
+  <si>
+    <t>0403 Capacitor</t>
+  </si>
+  <si>
     <t>D1</t>
   </si>
   <si>
@@ -548,7 +557,7 @@
     <t>Low Power Voltage Reference SOT23-3</t>
   </si>
   <si>
-    <t>ISL60002BIH318Z-TKCT-ND </t>
+    <t>ISL60002BIH318Z-TKCT-ND</t>
   </si>
   <si>
     <t>U7</t>
@@ -561,6 +570,18 @@
   </si>
   <si>
     <t>Three Electrod Gas Sensor</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>SI7021</t>
+  </si>
+  <si>
+    <t>DFN-6</t>
+  </si>
+  <si>
+    <t>Humidity Sensor</t>
   </si>
   <si>
     <t>X1</t>
@@ -605,6 +626,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -686,10 +708,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F59" activeCellId="0" sqref="F59"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1198,92 +1220,98 @@
         <v>62</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="E25" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>66</v>
-      </c>
       <c r="F25" s="0" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="E26" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>66</v>
-      </c>
       <c r="F27" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F28" s="0" t="s">
         <v>70</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="E29" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="C29" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="D29" s="0" t="s">
+      <c r="F29" s="0" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1291,61 +1319,61 @@
       <c r="A30" s="0" t="s">
         <v>78</v>
       </c>
+      <c r="B30" s="0" t="s">
+        <v>79</v>
+      </c>
       <c r="C30" s="0" t="s">
         <v>79</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="E30" s="0" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="D31" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="E31" s="0" t="s">
         <v>84</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="C32" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="D32" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F32" s="0" t="s">
         <v>88</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="D33" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="C33" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="D33" s="0" t="s">
+      <c r="F33" s="0" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1362,88 +1390,82 @@
       <c r="D34" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="E34" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="B35" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>96</v>
-      </c>
       <c r="E35" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E36" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="B36" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>97</v>
-      </c>
       <c r="F36" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="F37" s="0" t="s">
         <v>101</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="F37" s="0" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D38" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="E38" s="0" t="s">
         <v>108</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>105</v>
       </c>
       <c r="F38" s="0" t="s">
         <v>109</v>
@@ -1454,59 +1476,59 @@
         <v>110</v>
       </c>
       <c r="B39" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="E39" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="C39" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="E39" s="0" t="s">
-        <v>105</v>
-      </c>
       <c r="F39" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B40" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="C40" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="E40" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="C40" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>105</v>
-      </c>
       <c r="F40" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="F41" s="0" t="s">
         <v>112</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="F41" s="0" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1517,13 +1539,13 @@
         <v>116</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F42" s="0" t="s">
         <v>117</v>
@@ -1534,39 +1556,39 @@
         <v>118</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B44" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="C44" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="F44" s="0" t="s">
         <v>120</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="F44" s="0" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1577,13 +1599,13 @@
         <v>123</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F45" s="0" t="s">
         <v>124</v>
@@ -1597,13 +1619,13 @@
         <v>126</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F46" s="0" t="s">
         <v>127</v>
@@ -1617,13 +1639,13 @@
         <v>129</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F47" s="0" t="s">
         <v>130</v>
@@ -1637,13 +1659,13 @@
         <v>132</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F48" s="0" t="s">
         <v>133</v>
@@ -1657,13 +1679,13 @@
         <v>135</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F49" s="0" t="s">
         <v>136</v>
@@ -1677,13 +1699,13 @@
         <v>138</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F50" s="0" t="s">
         <v>139</v>
@@ -1697,13 +1719,13 @@
         <v>141</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F51" s="0" t="s">
         <v>142</v>
@@ -1717,196 +1739,233 @@
         <v>144</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>144</v>
+        <v>106</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>144</v>
+        <v>107</v>
       </c>
       <c r="E52" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="F52" s="0" t="s">
         <v>145</v>
-      </c>
-      <c r="F52" s="0" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B53" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="C53" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="E53" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="C53" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="D53" s="0" t="s">
+      <c r="F53" s="0" t="s">
         <v>149</v>
-      </c>
-      <c r="E53" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="F53" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="G53" s="0" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="E54" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="F54" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="C54" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="D54" s="0" t="s">
+      <c r="G54" s="0" t="s">
         <v>155</v>
-      </c>
-      <c r="E54" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="F54" s="0" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D55" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="B55" s="0" t="s">
+      <c r="E55" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="C55" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="D55" s="0" t="s">
+      <c r="F55" s="0" t="s">
         <v>160</v>
-      </c>
-      <c r="E55" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="F55" s="0" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D56" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="B56" s="0" t="s">
+      <c r="E56" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="C56" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="D56" s="0" t="s">
+      <c r="F56" s="0" t="s">
         <v>165</v>
-      </c>
-      <c r="E56" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="F56" s="0" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="D57" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="B57" s="0" t="s">
+      <c r="E57" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="C57" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="D57" s="0" t="s">
+      <c r="F57" s="0" t="s">
         <v>170</v>
-      </c>
-      <c r="E57" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="F57" s="0" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="D58" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="B58" s="0" t="s">
+      <c r="E58" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="C58" s="0" t="s">
+      <c r="F58" s="0" t="s">
         <v>175</v>
-      </c>
-      <c r="D58" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="E58" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="F58" s="0" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="C59" s="0" t="s">
         <v>178</v>
       </c>
-      <c r="B59" s="0" t="s">
+      <c r="D59" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="E59" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="C59" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="D59" s="0" t="s">
+      <c r="F59" s="0" t="s">
         <v>180</v>
-      </c>
-      <c r="E59" s="0" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B60" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="B60" s="0" t="s">
+      <c r="C60" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="D60" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="C60" s="0" t="s">
+      <c r="E60" s="0" t="s">
         <v>184</v>
-      </c>
-      <c r="D60" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="E60" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="F60" s="0" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="D61" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="B61" s="0" t="s">
+      <c r="E61" s="0" t="s">
         <v>188</v>
       </c>
-      <c r="C61" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="D61" s="0" t="s">
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="E61" s="0" t="s">
+      <c r="B62" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="F61" s="0" t="s">
+      <c r="C62" s="0" t="s">
         <v>191</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="F62" s="0" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="F63" s="0" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>